<commit_message>
format update in spreadsheet
</commit_message>
<xml_diff>
--- a/registries/Registry_of_metadata_tools_and_resources.xlsx
+++ b/registries/Registry_of_metadata_tools_and_resources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\IBASTRAK\ICSM MWG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\W10Dev\git\metadata-working-group\registries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,12 +165,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -224,9 +218,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -512,7 +503,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +515,7 @@
     <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -585,14 +576,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">

</xml_diff>